<commit_message>
Shop Service V2 (update, delete)
</commit_message>
<xml_diff>
--- a/SpMVC_ShopV2/쇼핑몰 테이블명세 양식.xlsx
+++ b/SpMVC_ShopV2/쇼핑몰 테이블명세 양식.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bizwork\workspace\spring\SpMVC_ShopV1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bizwork\workspace\spring\SpMVC_ShopV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
   <si>
     <t>열 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -285,6 +285,30 @@
   </si>
   <si>
     <t>NOT NULL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_NOT_USE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR(1)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열형</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제Flag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>값이 1이면 사용안함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D_NOT_USE</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -556,7 +580,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -621,6 +645,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -997,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:L3"/>
+    <sheetView showGridLines="0" topLeftCell="E4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1654,23 +1681,23 @@
       <c r="C1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="29" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="29"/>
+      <c r="I1" s="30"/>
       <c r="J1" s="13">
         <v>44062</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="31"/>
+      <c r="L1" s="32"/>
     </row>
     <row r="2" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="16" t="s">
@@ -1679,38 +1706,38 @@
       <c r="C2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="30" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="30"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="28"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
@@ -1916,16 +1943,26 @@
       <c r="B12" s="10">
         <v>8</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="19"/>
+      <c r="L12" s="19" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10">
@@ -2067,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2724,23 +2761,23 @@
       <c r="C1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="29" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="29"/>
+      <c r="I1" s="30"/>
       <c r="J1" s="13">
         <v>44062</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="31"/>
+      <c r="L1" s="32"/>
     </row>
     <row r="2" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="16" t="s">
@@ -2749,38 +2786,38 @@
       <c r="C2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="30" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="30"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="28"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
@@ -2988,16 +3025,26 @@
       <c r="B12" s="10">
         <v>8</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="C12" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="22"/>
+      <c r="L12" s="23" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10">
@@ -3121,12 +3168,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C3:L3"/>
     <mergeCell ref="D1:G2"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="C3:L3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>